<commit_message>
backing up files with csv and xlsx formats, along with reviewing data
</commit_message>
<xml_diff>
--- a/playstation/output/complete_database.xlsx
+++ b/playstation/output/complete_database.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="complete_database" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">complete_database!$A$1:$I$942</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">complete_database!$A$1:$I$944</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3773" uniqueCount="1520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="1525">
   <si>
     <t>ID</t>
   </si>
@@ -4573,6 +4573,21 @@
   </si>
   <si>
     <t>SouthPAW Games</t>
+  </si>
+  <si>
+    <t>Fallout Shelter</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -4583,7 +4598,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="[$€]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4605,8 +4620,14 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4619,6 +4640,24 @@
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -4626,7 +4665,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4646,6 +4685,21 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4866,6 +4920,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="40.75"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -48200,15 +48257,33 @@
       <c r="Z942" s="2"/>
     </row>
     <row r="943">
-      <c r="A943" s="2"/>
-      <c r="B943" s="2"/>
-      <c r="C943" s="2"/>
-      <c r="D943" s="2"/>
-      <c r="E943" s="2"/>
-      <c r="F943" s="2"/>
-      <c r="G943" s="2"/>
-      <c r="H943" s="2"/>
-      <c r="I943" s="2"/>
+      <c r="A943" s="3">
+        <v>942.0</v>
+      </c>
+      <c r="B943" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C943" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D943" s="4">
+        <v>45423.0</v>
+      </c>
+      <c r="E943" s="5">
+        <v>6.96</v>
+      </c>
+      <c r="F943" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G943" s="5">
+        <v>6.96</v>
+      </c>
+      <c r="H943" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="I943" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="J943" s="2"/>
       <c r="K943" s="2"/>
       <c r="L943" s="2"/>
@@ -48228,15 +48303,33 @@
       <c r="Z943" s="2"/>
     </row>
     <row r="944">
-      <c r="A944" s="2"/>
-      <c r="B944" s="2"/>
-      <c r="C944" s="2"/>
-      <c r="D944" s="2"/>
-      <c r="E944" s="2"/>
-      <c r="F944" s="2"/>
-      <c r="G944" s="2"/>
-      <c r="H944" s="2"/>
-      <c r="I944" s="2"/>
+      <c r="A944" s="3">
+        <v>943.0</v>
+      </c>
+      <c r="B944" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C944" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D944" s="4">
+        <v>45427.0</v>
+      </c>
+      <c r="E944" s="5">
+        <v>18.99</v>
+      </c>
+      <c r="F944" s="5">
+        <v>8.46</v>
+      </c>
+      <c r="G944" s="5">
+        <v>10.53</v>
+      </c>
+      <c r="H944" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="I944" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="J944" s="2"/>
       <c r="K944" s="2"/>
       <c r="L944" s="2"/>
@@ -48288,13 +48381,31 @@
       <c r="B946" s="2"/>
       <c r="C946" s="2"/>
       <c r="D946" s="2"/>
-      <c r="E946" s="2"/>
-      <c r="F946" s="2"/>
-      <c r="G946" s="2"/>
-      <c r="H946" s="2"/>
-      <c r="I946" s="2"/>
-      <c r="J946" s="2"/>
-      <c r="K946" s="2"/>
+      <c r="E946" s="7">
+        <f t="shared" ref="E946:G946" si="1">SUM(E2:E944)</f>
+        <v>22819.62</v>
+      </c>
+      <c r="F946" s="8">
+        <f t="shared" si="1"/>
+        <v>10205.15</v>
+      </c>
+      <c r="G946" s="9">
+        <f t="shared" si="1"/>
+        <v>12614.47</v>
+      </c>
+      <c r="H946" s="10">
+        <f>COUNTA(A2:A944)</f>
+        <v>943</v>
+      </c>
+      <c r="I946" s="11" t="s">
+        <v>1522</v>
+      </c>
+      <c r="J946" s="11">
+        <v>16.0</v>
+      </c>
+      <c r="K946" s="11" t="s">
+        <v>1523</v>
+      </c>
       <c r="L946" s="2"/>
       <c r="M946" s="2"/>
       <c r="N946" s="2"/>
@@ -48316,13 +48427,32 @@
       <c r="B947" s="2"/>
       <c r="C947" s="2"/>
       <c r="D947" s="2"/>
-      <c r="E947" s="2"/>
-      <c r="F947" s="2"/>
-      <c r="G947" s="2"/>
-      <c r="H947" s="2"/>
-      <c r="I947" s="2"/>
-      <c r="J947" s="2"/>
-      <c r="K947" s="2"/>
+      <c r="E947" s="7">
+        <f>E946/J946</f>
+        <v>1426.22625</v>
+      </c>
+      <c r="F947" s="8">
+        <f>F946/J946</f>
+        <v>637.821875</v>
+      </c>
+      <c r="G947" s="9">
+        <f>G946/J946</f>
+        <v>788.404375</v>
+      </c>
+      <c r="H947" s="10">
+        <f>H946/J946</f>
+        <v>58.9375</v>
+      </c>
+      <c r="I947" s="11" t="s">
+        <v>1522</v>
+      </c>
+      <c r="J947" s="10">
+        <f>J946/J946</f>
+        <v>1</v>
+      </c>
+      <c r="K947" s="11" t="s">
+        <v>1524</v>
+      </c>
       <c r="L947" s="2"/>
       <c r="M947" s="2"/>
       <c r="N947" s="2"/>
@@ -49851,8 +49981,64 @@
       <c r="Y1001" s="2"/>
       <c r="Z1001" s="2"/>
     </row>
+    <row r="1002">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="2"/>
+      <c r="C1002" s="2"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="2"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="2"/>
+      <c r="M1002" s="2"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+      <c r="R1002" s="2"/>
+      <c r="S1002" s="2"/>
+      <c r="T1002" s="2"/>
+      <c r="U1002" s="2"/>
+      <c r="V1002" s="2"/>
+      <c r="W1002" s="2"/>
+      <c r="X1002" s="2"/>
+      <c r="Y1002" s="2"/>
+      <c r="Z1002" s="2"/>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$I$942"/>
+  <autoFilter ref="$A$1:$I$944"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H695"/>
     <hyperlink r:id="rId2" ref="H897"/>

</xml_diff>